<commit_message>
Various spreadsheet changes - see comment in PR
</commit_message>
<xml_diff>
--- a/data/agage/data_exclude.xlsx
+++ b/data/agage/data_exclude.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOEPIT~1\AppData\Local\Temp\scp43046\user\home\zh21490\agage-archive\data\agage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B39A74-B040-438C-9052-B2CD7AEAA8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA58694-107B-4019-8D68-84E327C2F9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ADR" sheetId="11" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="CMN" sheetId="5" r:id="rId3"/>
     <sheet name="CMO" sheetId="9" r:id="rId4"/>
     <sheet name="GSN" sheetId="7" r:id="rId5"/>
-    <sheet name="MHD" sheetId="4" r:id="rId6"/>
-    <sheet name="SMO" sheetId="10" r:id="rId7"/>
+    <sheet name="SMO" sheetId="10" r:id="rId6"/>
+    <sheet name="MHD" sheetId="4" r:id="rId7"/>
     <sheet name="RPB" sheetId="8" r:id="rId8"/>
     <sheet name="TAC" sheetId="12" r:id="rId9"/>
     <sheet name="THD" sheetId="3" r:id="rId10"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3374" uniqueCount="1012">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="1017">
   <si>
     <t>Species</t>
   </si>
@@ -3082,6 +3082,21 @@
   </si>
   <si>
     <t>2023-08-22 00:01</t>
+  </si>
+  <si>
+    <t>2023-05-17 00:00</t>
+  </si>
+  <si>
+    <t>cf4</t>
+  </si>
+  <si>
+    <t>2022-04-20 00:00</t>
+  </si>
+  <si>
+    <t>2022-12-10 00:00</t>
+  </si>
+  <si>
+    <t>From Ray Wang's table</t>
   </si>
 </sst>
 </file>
@@ -4130,10 +4145,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4179,6 +4194,21 @@
         <v>107</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4186,10 +4216,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E148"/>
+  <dimension ref="A1:E149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6678,6 +6708,23 @@
         <v>108</v>
       </c>
     </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>1016</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6687,8 +6734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="F91" sqref="F91"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6739,7 +6786,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>989</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -6753,7 +6800,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>989</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
@@ -6767,7 +6814,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>989</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
@@ -9694,6 +9741,1400 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:E83"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.875" style="1"/>
+    <col min="3" max="4" width="15.5" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="E6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="E7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="E8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="E10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="E11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="E12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="E13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="E14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="E15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="E16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="E17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="E18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="E19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="E21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="E22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="E23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="E24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="E25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="E26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="E27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="E28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="E29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="E31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="E32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="E33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="E34" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="E35" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="E36" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="E37" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E38" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="E39" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="E40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="E41" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="E42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="E43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="E44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="E45" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="E46" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="E47" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="E48" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="E49" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="E50" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="E51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E52" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="E53" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="E54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="E55" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="E56" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="E57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="E58" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="E59" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="E60" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="E61" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="E62" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E63" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="E64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="E65" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="E66" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="E67" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="E68" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="E69" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="E70" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="E71" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="E72" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="E73" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="E74" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="E75" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="E76" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="E77" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="E78" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="E79" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="E80" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="E81" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="E82" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E83" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E60"/>
   <sheetViews>
@@ -10690,1400 +12131,6 @@
         <v>391</v>
       </c>
       <c r="E60" t="s">
-        <v>108</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E83"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="10.875" style="1"/>
-    <col min="3" max="4" width="15.5" style="1" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="E6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>655</v>
-      </c>
-      <c r="E7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>657</v>
-      </c>
-      <c r="E8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="E10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>660</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="E11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="E12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="E13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="E14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>668</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="E15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>670</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="E16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>672</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="E17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>674</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="E18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>676</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>677</v>
-      </c>
-      <c r="E19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="E21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>679</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>680</v>
-      </c>
-      <c r="E22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>681</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="E23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>684</v>
-      </c>
-      <c r="E24" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>686</v>
-      </c>
-      <c r="E25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="E26" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="E27" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>692</v>
-      </c>
-      <c r="E28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>694</v>
-      </c>
-      <c r="E29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="E31" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="E32" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>697</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="E33" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="E34" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>702</v>
-      </c>
-      <c r="E35" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>703</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>704</v>
-      </c>
-      <c r="E36" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>705</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="E37" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E38" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>708</v>
-      </c>
-      <c r="E39" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="E40" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>709</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="E41" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="E42" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="E43" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>715</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>716</v>
-      </c>
-      <c r="E44" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>717</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>718</v>
-      </c>
-      <c r="E45" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>719</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>720</v>
-      </c>
-      <c r="E46" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>721</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>722</v>
-      </c>
-      <c r="E47" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>723</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="E48" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>725</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>726</v>
-      </c>
-      <c r="E49" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>727</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="E50" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>729</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="E51" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E52" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>732</v>
-      </c>
-      <c r="E53" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="E54" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>733</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="E55" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="E56" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="E57" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>668</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="E58" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>670</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="E59" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>737</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>738</v>
-      </c>
-      <c r="E60" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="E61" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>742</v>
-      </c>
-      <c r="E62" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>743</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E63" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>744</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="E64" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="E65" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>746</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>747</v>
-      </c>
-      <c r="E66" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>749</v>
-      </c>
-      <c r="E67" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>750</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="E68" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>752</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="E69" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>754</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>755</v>
-      </c>
-      <c r="E70" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>756</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>757</v>
-      </c>
-      <c r="E71" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>758</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>759</v>
-      </c>
-      <c r="E72" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>760</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>761</v>
-      </c>
-      <c r="E73" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>763</v>
-      </c>
-      <c r="E74" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>764</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>765</v>
-      </c>
-      <c r="E75" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>766</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>767</v>
-      </c>
-      <c r="E76" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>768</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>769</v>
-      </c>
-      <c r="E77" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>770</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>771</v>
-      </c>
-      <c r="E78" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>772</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>773</v>
-      </c>
-      <c r="E79" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>774</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="E80" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>776</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="E81" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>778</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>779</v>
-      </c>
-      <c r="E82" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E83" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>